<commit_message>
Adding references to structure searching section
</commit_message>
<xml_diff>
--- a/01_DATA/Amidase_3/00_BasicStructureSearch_PossibleAmidaseLonglist/00_NAMLA amidase family_structures_2023_all_PDB.xlsx
+++ b/01_DATA/Amidase_3/00_BasicStructureSearch_PossibleAmidaseLonglist/00_NAMLA amidase family_structures_2023_all_PDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\OneDrive - Birkbeck, University of London\Birkbeck MSc\MSc Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MSc_Project\MSc_Project\01_DATA\Amidase_3\00_BasicStructureSearch_PossibleAmidaseLonglist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93D30C2-A1F0-49A6-A823-604CB312FEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283724F6-491F-4D9F-8D31-B32B448BBAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="2175" windowWidth="18525" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9780" yWindow="4725" windowWidth="18525" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PDB Structures" sheetId="2" r:id="rId1"/>
@@ -4540,8 +4540,8 @@
   <dimension ref="A1:AN237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4551,7 +4551,7 @@
     <col min="3" max="3" width="5.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60.140625" style="10" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="10" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.28515625" style="10" customWidth="1"/>
     <col min="9" max="9" width="63.42578125" style="10" customWidth="1"/>

</xml_diff>